<commit_message>
(U)    update to routine of D2
</commit_message>
<xml_diff>
--- a/Suppl/Thrive Fitness Plan - Lifting - heh.xlsx
+++ b/Suppl/Thrive Fitness Plan - Lifting - heh.xlsx
@@ -171,9 +171,6 @@
     <t>Shoulders &amp; Traps</t>
   </si>
   <si>
-    <t>Dumbbell Flat Bench Press</t>
-  </si>
-  <si>
     <t>Barbbell Shoulder Press</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>Kettlebell Squat-to-Upright Row</t>
   </si>
   <si>
-    <t>Dumbell Incline Bench Press</t>
-  </si>
-  <si>
     <t>Hanging Leg Raises</t>
   </si>
   <si>
@@ -250,6 +244,12 @@
   </si>
   <si>
     <t>16/16/10</t>
+  </si>
+  <si>
+    <t>Dumbbell Incline Bench Press</t>
+  </si>
+  <si>
+    <t>Dumbell Flat Bench Press</t>
   </si>
 </sst>
 </file>
@@ -746,7 +746,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1055,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1066,7 +1066,7 @@
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="19"/>
@@ -1112,17 +1112,17 @@
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="25" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
       <c r="E19" s="26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="27"/>
       <c r="H19" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
@@ -1133,17 +1133,17 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="27"/>
       <c r="H20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
@@ -1154,7 +1154,7 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="25" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -1164,7 +1164,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="31"/>
       <c r="H21" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
@@ -1175,17 +1175,17 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="E22" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="27"/>
       <c r="H22" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
@@ -1196,7 +1196,7 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -1206,18 +1206,18 @@
       <c r="F23" s="2"/>
       <c r="G23" s="27"/>
       <c r="H23" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I23" s="28"/>
       <c r="J23" s="28"/>
       <c r="K23" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
       <c r="B24" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
@@ -1227,39 +1227,39 @@
       <c r="F24" s="2"/>
       <c r="G24" s="27"/>
       <c r="H24" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="30"/>
       <c r="B25" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
       <c r="E25" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="31"/>
       <c r="H25" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I25" s="28"/>
       <c r="J25" s="28"/>
       <c r="K25" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
@@ -1269,7 +1269,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="31"/>
       <c r="H26" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I26" s="28"/>
       <c r="J26" s="28"/>
@@ -1280,7 +1280,7 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
@@ -1290,12 +1290,12 @@
       <c r="F27" s="2"/>
       <c r="G27" s="31"/>
       <c r="H27" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I27" s="28"/>
       <c r="J27" s="28"/>
       <c r="K27" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
(U)    workout plan updates
</commit_message>
<xml_diff>
--- a/Suppl/Thrive Fitness Plan - Lifting - heh.xlsx
+++ b/Suppl/Thrive Fitness Plan - Lifting - heh.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>Plan</t>
   </si>
@@ -81,15 +81,9 @@
     <t>12/12/12</t>
   </si>
   <si>
-    <t>Seated Hammer Curls</t>
-  </si>
-  <si>
     <t>8/12/12</t>
   </si>
   <si>
-    <t>Wide Grip Lat Pulldowns, Slow</t>
-  </si>
-  <si>
     <t>10/12/12</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>Medicine Ball Pushups</t>
   </si>
   <si>
-    <t>8/8/8/8</t>
-  </si>
-  <si>
     <t>Kettlebell Squat-to-Upright Row</t>
   </si>
   <si>
@@ -204,9 +195,6 @@
     <t>12/10/8</t>
   </si>
   <si>
-    <t>12/12/15</t>
-  </si>
-  <si>
     <t>15/20/20</t>
   </si>
   <si>
@@ -238,6 +226,18 @@
   </si>
   <si>
     <t>16/16/16</t>
+  </si>
+  <si>
+    <t>Hammer Curl, Seated</t>
+  </si>
+  <si>
+    <t>Wide Grip Lat Pulldown, Slow</t>
+  </si>
+  <si>
+    <t>12/10/10</t>
+  </si>
+  <si>
+    <t>Single Arm Dumbbell Rows</t>
   </si>
 </sst>
 </file>
@@ -453,18 +453,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,13 +751,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K28" sqref="A1:K28"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="11" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="11" style="36" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -782,10 +787,10 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="35">
         <v>42793</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="1"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -856,102 +861,102 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="15"/>
       <c r="H6" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="38" t="s">
-        <v>69</v>
+      <c r="K6" s="34" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13" t="s">
-        <v>16</v>
+      <c r="B7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="37" t="s">
+        <v>21</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="15"/>
       <c r="H7" s="19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="37" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13" t="s">
-        <v>21</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="19"/>
       <c r="H8" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
-        <v>23</v>
+        <v>61</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="19"/>
       <c r="H9" s="16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="15"/>
       <c r="H10" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
@@ -960,116 +965,112 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="15"/>
       <c r="H11" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="13" t="s">
-        <v>19</v>
+      <c r="E12" s="37" t="s">
+        <v>30</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="19"/>
       <c r="H12" s="16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
-      <c r="K12" s="38" t="s">
-        <v>23</v>
+      <c r="K12" s="34" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="13" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="19"/>
       <c r="H13" s="16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
-      <c r="K13" s="38" t="s">
+      <c r="K13" s="34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="21"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="37" t="s">
+        <v>19</v>
+      </c>
       <c r="F14" s="14"/>
       <c r="G14" s="15"/>
       <c r="H14" s="16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="10"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="14"/>
       <c r="G15" s="15"/>
       <c r="H15" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
-      <c r="K15" s="38" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="25" t="s">
-        <v>16</v>
-      </c>
+      <c r="K15" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="14"/>
       <c r="G16" s="19"/>
       <c r="H16" s="16"/>
@@ -1077,16 +1078,16 @@
       <c r="J16" s="16"/>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="25" t="s">
-        <v>42</v>
-      </c>
+    <row r="17" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="5"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1095,40 +1096,40 @@
       <c r="K17" s="22"/>
     </row>
     <row r="18" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
-      <c r="B18" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="25" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="25" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="26"/>
       <c r="H19" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
@@ -1137,19 +1138,19 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="26"/>
       <c r="H20" s="27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="27"/>
@@ -1158,19 +1159,19 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="25" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="30"/>
       <c r="H21" s="27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
@@ -1180,18 +1181,18 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
-      <c r="B22" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
+      <c r="B22" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="25" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="26"/>
       <c r="H22" s="27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I22" s="27"/>
       <c r="J22" s="27"/>
@@ -1200,57 +1201,61 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="26"/>
       <c r="H23" s="27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
       <c r="K23" s="28" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
-      <c r="B24" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="B24" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="30"/>
       <c r="H24" s="27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I24" s="27"/>
       <c r="J24" s="27"/>
       <c r="K24" s="28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="32" t="s">
+        <v>55</v>
+      </c>
       <c r="C25" s="32"/>
       <c r="D25" s="32"/>
-      <c r="E25" s="33"/>
+      <c r="E25" s="25" t="s">
+        <v>19</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="30"/>
       <c r="H25" s="27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
@@ -1259,27 +1264,34 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="38"/>
+      <c r="B26" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="2"/>
       <c r="G26" s="26"/>
       <c r="H26" s="27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
       <c r="K26" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F27" s="2"/>
       <c r="G27" s="26"/>
       <c r="H27" s="27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I27" s="27"/>
       <c r="J27" s="27"/>
       <c r="K27" s="28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>